<commit_message>
- Added all available streams (and their categories). - Ensured streams are always grouped by their category.. - Removed legacy stream controls.
</commit_message>
<xml_diff>
--- a/app/assets/data/staff-details.xlsx
+++ b/app/assets/data/staff-details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\cip-nightapps-prototype\app\assets\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C07AC13F-4F83-44C3-BC8F-9B424347292A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34D3A40A-4B50-4A78-BE20-9BFC0C0DB6A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C6DB01E0-F7B1-4D21-83EC-2E65691F7497}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Staff Details" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Staff Details'!$A$2:$AD$5</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Staff Details'!$A$2:$AI$5</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="82">
   <si>
     <t>Surname</t>
   </si>
@@ -149,12 +149,6 @@
     <t>No</t>
   </si>
   <si>
-    <t>Item Confirmation, Submission Correction, Multiple Hits, Errors, Quantity Validation, PECS</t>
-  </si>
-  <si>
-    <t>PECS</t>
-  </si>
-  <si>
     <t>Forename</t>
   </si>
   <si>
@@ -245,12 +239,6 @@
     <t>Office Worker</t>
   </si>
   <si>
-    <t>Multiple Hits, Errors, Quantity Validation</t>
-  </si>
-  <si>
-    <t>Assigned Streams</t>
-  </si>
-  <si>
     <t>Individual Details</t>
   </si>
   <si>
@@ -258,6 +246,45 @@
   </si>
   <si>
     <t>Status</t>
+  </si>
+  <si>
+    <t>Production</t>
+  </si>
+  <si>
+    <t>Prescription Scanning</t>
+  </si>
+  <si>
+    <t>Legacy</t>
+  </si>
+  <si>
+    <t>Portering</t>
+  </si>
+  <si>
+    <t>Student Services</t>
+  </si>
+  <si>
+    <t>Scanning Services</t>
+  </si>
+  <si>
+    <t>Islands Account, Islands Reconciliation</t>
+  </si>
+  <si>
+    <t>Bailing</t>
+  </si>
+  <si>
+    <t>Item Confirmation</t>
+  </si>
+  <si>
+    <t>Scan Applications, Scan CCR</t>
+  </si>
+  <si>
+    <t>PADM - Docketing, PADM - Scanning</t>
+  </si>
+  <si>
+    <t>Applications</t>
+  </si>
+  <si>
+    <t>BTST</t>
   </si>
 </sst>
 </file>
@@ -657,7 +684,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED5AB09E-8427-43CE-A5E4-2EA0450F5516}">
-  <dimension ref="A1:AD5"/>
+  <dimension ref="A1:AI5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection sqref="A1:F1"/>
@@ -691,13 +718,13 @@
     <col min="27" max="27" width="10.28515625" style="2" customWidth="1"/>
     <col min="28" max="28" width="13" style="2" customWidth="1"/>
     <col min="29" max="29" width="16.140625" style="2" customWidth="1"/>
-    <col min="30" max="30" width="82.7109375" style="2" customWidth="1"/>
-    <col min="31" max="16384" width="9.140625" style="2"/>
+    <col min="30" max="35" width="40.7109375" style="2" customWidth="1"/>
+    <col min="36" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:30" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="B1" s="7"/>
       <c r="C1" s="7"/>
@@ -705,13 +732,13 @@
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
       <c r="G1" s="7" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="H1" s="7"/>
       <c r="I1" s="7"/>
       <c r="J1" s="7"/>
       <c r="K1" s="7" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="L1" s="7"/>
       <c r="M1" s="7"/>
@@ -739,7 +766,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:30" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
@@ -750,22 +777,22 @@
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I2" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>5</v>
@@ -774,22 +801,22 @@
         <v>4</v>
       </c>
       <c r="L2" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="N2" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="M2" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="N2" s="1" t="s">
+      <c r="O2" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="O2" s="1" t="s">
+      <c r="P2" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="P2" s="1" t="s">
-        <v>61</v>
-      </c>
       <c r="Q2" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="R2" s="1" t="s">
         <v>8</v>
@@ -830,8 +857,23 @@
       <c r="AD2" s="1" t="s">
         <v>69</v>
       </c>
+      <c r="AE2" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="AF2" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="AG2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="AH2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="AI2" s="1" t="s">
+        <v>74</v>
+      </c>
     </row>
-    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>31</v>
       </c>
@@ -848,31 +890,31 @@
         <v>25</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="I3" s="4" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="L3" s="3">
         <v>43831</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="R3" s="3">
         <v>43831</v>
@@ -902,10 +944,16 @@
         <v>7.5</v>
       </c>
       <c r="AD3" s="2" t="s">
-        <v>36</v>
+        <v>75</v>
+      </c>
+      <c r="AF3" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="AG3" s="2" t="s">
+        <v>76</v>
       </c>
     </row>
-    <row r="4" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>32</v>
       </c>
@@ -919,37 +967,37 @@
         <v>23</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>26</v>
       </c>
       <c r="G4" s="2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="H4" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="I4" s="4" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="J4" s="2" t="s">
         <v>6</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="L4" s="3">
         <v>44197</v>
       </c>
       <c r="O4" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="P4" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="P4" s="3" t="s">
-        <v>65</v>
-      </c>
       <c r="Q4" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="R4" s="3">
         <v>43831</v>
@@ -979,10 +1027,13 @@
         <v>7.5</v>
       </c>
       <c r="AD4" s="2" t="s">
-        <v>68</v>
+        <v>77</v>
+      </c>
+      <c r="AH4" s="2" t="s">
+        <v>78</v>
       </c>
     </row>
-    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>33</v>
       </c>
@@ -999,19 +1050,19 @@
         <v>27</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="I5" s="4" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="J5" s="2" t="s">
         <v>7</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="L5" s="3">
         <v>45292</v>
@@ -1020,16 +1071,16 @@
         <v>45658</v>
       </c>
       <c r="N5" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="P5" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q5" s="3" t="s">
         <v>65</v>
-      </c>
-      <c r="Q5" s="3" t="s">
-        <v>67</v>
       </c>
       <c r="R5" s="3">
         <v>43831</v>
@@ -1061,12 +1112,15 @@
       <c r="AA5" s="2">
         <v>4</v>
       </c>
-      <c r="AD5" s="2" t="s">
-        <v>37</v>
+      <c r="AE5" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="AF5" s="2" t="s">
+        <v>80</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:AD5" xr:uid="{ED5AB09E-8427-43CE-A5E4-2EA0450F5516}"/>
+  <autoFilter ref="A2:AI5" xr:uid="{ED5AB09E-8427-43CE-A5E4-2EA0450F5516}"/>
   <mergeCells count="5">
     <mergeCell ref="W1:AC1"/>
     <mergeCell ref="A1:F1"/>

</xml_diff>

<commit_message>
- Fixed staff details download to match current data expectations.
</commit_message>
<xml_diff>
--- a/app/assets/data/staff-details.xlsx
+++ b/app/assets/data/staff-details.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\cip-nightapps-prototype\app\assets\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34D3A40A-4B50-4A78-BE20-9BFC0C0DB6A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5626C01-9A25-4DC9-8A98-3AC88103A159}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C6DB01E0-F7B1-4D21-83EC-2E65691F7497}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="74">
   <si>
     <t>Surname</t>
   </si>
@@ -53,9 +53,6 @@
     <t>Payroll Number</t>
   </si>
   <si>
-    <t>Status Group</t>
-  </si>
-  <si>
     <t>Shift Pattern</t>
   </si>
   <si>
@@ -110,39 +107,6 @@
     <t>Role</t>
   </si>
   <si>
-    <t>Paul</t>
-  </si>
-  <si>
-    <t>Tony</t>
-  </si>
-  <si>
-    <t>Smith</t>
-  </si>
-  <si>
-    <t>Jones</t>
-  </si>
-  <si>
-    <t>Robinson</t>
-  </si>
-  <si>
-    <t>pasmi</t>
-  </si>
-  <si>
-    <t>pajon</t>
-  </si>
-  <si>
-    <t>torob</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 	paul.smith@nhs.net </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 	paul.jones@nhs.net </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 	tony.robinson@nhs.net</t>
-  </si>
-  <si>
     <t>Yes</t>
   </si>
   <si>
@@ -155,9 +119,6 @@
     <t>Middle Name(s)</t>
   </si>
   <si>
-    <t>James-Andrew</t>
-  </si>
-  <si>
     <t>Manager Name</t>
   </si>
   <si>
@@ -167,48 +128,12 @@
     <t>Manager E-mail</t>
   </si>
   <si>
-    <t>Demo Manager 1</t>
-  </si>
-  <si>
-    <t>Demo Manager 2</t>
-  </si>
-  <si>
-    <t>Demo Manager 3</t>
-  </si>
-  <si>
-    <t>deman1</t>
-  </si>
-  <si>
-    <t>deman2</t>
-  </si>
-  <si>
-    <t>deman3</t>
-  </si>
-  <si>
-    <t>demo.manager1@nhs.net</t>
-  </si>
-  <si>
-    <t>demo.manager2@nhs.net</t>
-  </si>
-  <si>
-    <t>demo.manager3@nhs.net</t>
-  </si>
-  <si>
     <t>Substantive</t>
   </si>
   <si>
     <t>Loan</t>
   </si>
   <si>
-    <t>Status Group - Start Date</t>
-  </si>
-  <si>
-    <t>Status Group - Finish Date</t>
-  </si>
-  <si>
-    <t>Status Group - Moved To</t>
-  </si>
-  <si>
     <t>Wakefield</t>
   </si>
   <si>
@@ -254,9 +179,6 @@
     <t>Prescription Scanning</t>
   </si>
   <si>
-    <t>Legacy</t>
-  </si>
-  <si>
     <t>Portering</t>
   </si>
   <si>
@@ -285,6 +207,60 @@
   </si>
   <si>
     <t>BTST</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> demo.staff1@nhs.net </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> demo.staff2@nhs.net </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> demo.staff3@nhs.net </t>
+  </si>
+  <si>
+    <t>desta1</t>
+  </si>
+  <si>
+    <t>desta2</t>
+  </si>
+  <si>
+    <t>desta3</t>
+  </si>
+  <si>
+    <t>Demo</t>
+  </si>
+  <si>
+    <t>Staff</t>
+  </si>
+  <si>
+    <t>Member1</t>
+  </si>
+  <si>
+    <t>Member2</t>
+  </si>
+  <si>
+    <t>Member3</t>
+  </si>
+  <si>
+    <t>Demo Manager</t>
+  </si>
+  <si>
+    <t>deman</t>
+  </si>
+  <si>
+    <t>demo.manager@nhs.net</t>
+  </si>
+  <si>
+    <t>Group</t>
+  </si>
+  <si>
+    <t>Finish Date</t>
+  </si>
+  <si>
+    <t>Moved To</t>
+  </si>
+  <si>
+    <t>SCS</t>
   </si>
 </sst>
 </file>
@@ -294,7 +270,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -312,14 +288,6 @@
     </font>
     <font>
       <sz val="8"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -342,9 +310,8 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -357,9 +324,6 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="2" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -369,9 +333,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -699,18 +663,18 @@
     <col min="5" max="5" width="19.85546875" style="2" customWidth="1"/>
     <col min="6" max="8" width="21.7109375" style="2" customWidth="1"/>
     <col min="9" max="9" width="33" style="2" customWidth="1"/>
-    <col min="10" max="10" width="24.7109375" style="2" customWidth="1"/>
-    <col min="11" max="11" width="24.85546875" style="2" customWidth="1"/>
-    <col min="12" max="12" width="27.85546875" style="3" customWidth="1"/>
-    <col min="13" max="13" width="27.7109375" style="3" customWidth="1"/>
-    <col min="14" max="14" width="38.28515625" style="2" customWidth="1"/>
-    <col min="15" max="15" width="30.7109375" style="2" customWidth="1"/>
-    <col min="16" max="17" width="23.5703125" style="2" customWidth="1"/>
-    <col min="18" max="18" width="20.42578125" style="2" customWidth="1"/>
-    <col min="19" max="19" width="9.85546875" style="6" customWidth="1"/>
-    <col min="20" max="20" width="22.140625" style="2" customWidth="1"/>
-    <col min="21" max="21" width="27.28515625" style="2" customWidth="1"/>
-    <col min="22" max="22" width="24.42578125" style="2" customWidth="1"/>
+    <col min="10" max="10" width="24.85546875" style="2" customWidth="1"/>
+    <col min="11" max="11" width="19.7109375" style="3" customWidth="1"/>
+    <col min="12" max="12" width="18.28515625" style="3" customWidth="1"/>
+    <col min="13" max="13" width="20.140625" style="2" customWidth="1"/>
+    <col min="14" max="14" width="30.7109375" style="2" customWidth="1"/>
+    <col min="15" max="16" width="23.5703125" style="2" customWidth="1"/>
+    <col min="17" max="17" width="20.42578125" style="2" customWidth="1"/>
+    <col min="18" max="18" width="9.85546875" style="5" customWidth="1"/>
+    <col min="19" max="19" width="22.140625" style="2" customWidth="1"/>
+    <col min="20" max="20" width="27.28515625" style="2" customWidth="1"/>
+    <col min="21" max="21" width="24.42578125" style="2" customWidth="1"/>
+    <col min="22" max="22" width="17" style="2" customWidth="1"/>
     <col min="23" max="23" width="11.7109375" style="2" customWidth="1"/>
     <col min="24" max="24" width="11.42578125" style="2" customWidth="1"/>
     <col min="25" max="25" width="13.85546875" style="2" customWidth="1"/>
@@ -723,47 +687,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" s="1" customFormat="1" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="7" t="s">
-        <v>66</v>
-      </c>
-      <c r="B1" s="7"/>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-      <c r="G1" s="7" t="s">
-        <v>67</v>
-      </c>
-      <c r="H1" s="7"/>
-      <c r="I1" s="7"/>
-      <c r="J1" s="7"/>
-      <c r="K1" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="L1" s="7"/>
-      <c r="M1" s="7"/>
-      <c r="N1" s="7"/>
-      <c r="O1" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="P1" s="7"/>
-      <c r="Q1" s="7"/>
-      <c r="R1" s="7"/>
-      <c r="S1" s="7"/>
-      <c r="T1" s="7"/>
-      <c r="U1" s="7"/>
-      <c r="V1" s="7"/>
-      <c r="W1" s="7" t="s">
+      <c r="A1" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="K1" s="6"/>
+      <c r="L1" s="6"/>
+      <c r="M1" s="6"/>
+      <c r="N1" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="X1" s="7"/>
-      <c r="Y1" s="7"/>
-      <c r="Z1" s="7"/>
-      <c r="AA1" s="7"/>
-      <c r="AB1" s="7"/>
-      <c r="AC1" s="7"/>
+      <c r="O1" s="6"/>
+      <c r="P1" s="6"/>
+      <c r="Q1" s="6"/>
+      <c r="R1" s="6"/>
+      <c r="S1" s="6"/>
+      <c r="T1" s="6"/>
+      <c r="U1" s="6"/>
+      <c r="V1" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="W1" s="6"/>
+      <c r="X1" s="6"/>
+      <c r="Y1" s="6"/>
+      <c r="Z1" s="6"/>
+      <c r="AA1" s="6"/>
+      <c r="AB1" s="6"/>
+      <c r="AC1" s="6"/>
       <c r="AD1" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:35" s="1" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -777,51 +741,51 @@
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>36</v>
+        <v>24</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>37</v>
+        <v>25</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>0</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>5</v>
+        <v>70</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>53</v>
+        <v>71</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>54</v>
+        <v>72</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>55</v>
+        <v>32</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>59</v>
+        <v>33</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="R2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="R2" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="S2" s="5" t="s">
+      <c r="S2" s="1" t="s">
         <v>9</v>
       </c>
       <c r="T2" s="1" t="s">
@@ -831,311 +795,311 @@
         <v>11</v>
       </c>
       <c r="V2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="W2" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="W2" s="1" t="s">
+      <c r="X2" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="X2" s="1" t="s">
+      <c r="Y2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="Y2" s="1" t="s">
+      <c r="Z2" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Z2" s="1" t="s">
+      <c r="AA2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="AA2" s="1" t="s">
+      <c r="AB2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="AB2" s="1" t="s">
+      <c r="AC2" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="AC2" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="AD2" s="1" t="s">
-        <v>69</v>
+        <v>44</v>
       </c>
       <c r="AE2" s="1" t="s">
-        <v>70</v>
+        <v>45</v>
       </c>
       <c r="AF2" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="AG2" s="1" t="s">
-        <v>72</v>
+        <v>46</v>
       </c>
       <c r="AH2" s="1" t="s">
-        <v>73</v>
+        <v>47</v>
       </c>
       <c r="AI2" s="1" t="s">
-        <v>74</v>
+        <v>48</v>
       </c>
     </row>
     <row r="3" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>31</v>
+        <v>56</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>28</v>
+        <v>59</v>
       </c>
       <c r="C3" s="2">
         <v>1000001</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>23</v>
+        <v>62</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>63</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>25</v>
+        <v>64</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>42</v>
+        <v>67</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="I3" s="4" t="s">
-        <v>48</v>
+        <v>68</v>
+      </c>
+      <c r="I3" s="7" t="s">
+        <v>69</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="L3" s="3">
+        <v>29</v>
+      </c>
+      <c r="K3" s="3">
         <v>43831</v>
       </c>
+      <c r="N3" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="O3" s="3" t="s">
-        <v>60</v>
+        <v>38</v>
       </c>
       <c r="P3" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q3" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="R3" s="3">
+        <v>39</v>
+      </c>
+      <c r="Q3" s="3">
         <v>43831</v>
       </c>
-      <c r="S3" s="6">
+      <c r="R3" s="5">
         <v>1</v>
       </c>
+      <c r="T3" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="U3" s="2" t="s">
-        <v>34</v>
+        <v>22</v>
       </c>
       <c r="V3" s="2" t="s">
-        <v>34</v>
+        <v>5</v>
       </c>
       <c r="W3" s="2">
-        <v>7.5</v>
+        <v>450</v>
       </c>
       <c r="X3" s="2">
-        <v>7.5</v>
+        <v>450</v>
       </c>
       <c r="Y3" s="2">
-        <v>7.5</v>
+        <v>450</v>
       </c>
       <c r="Z3" s="2">
-        <v>7.5</v>
+        <v>450</v>
       </c>
       <c r="AA3" s="2">
-        <v>7.5</v>
+        <v>450</v>
       </c>
       <c r="AD3" s="2" t="s">
-        <v>75</v>
+        <v>49</v>
       </c>
       <c r="AF3" s="2" t="s">
-        <v>81</v>
+        <v>55</v>
       </c>
       <c r="AG3" s="2" t="s">
-        <v>76</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>32</v>
+        <v>57</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>29</v>
+        <v>60</v>
       </c>
       <c r="C4" s="2">
         <v>1000002</v>
       </c>
       <c r="D4" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I4" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="K4" s="3">
+        <v>44197</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="O4" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="Q4" s="3">
+        <v>43831</v>
+      </c>
+      <c r="R4" s="5">
+        <v>1</v>
+      </c>
+      <c r="T4" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="F4" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G4" s="2" t="s">
-        <v>43</v>
-      </c>
-      <c r="H4" s="2" t="s">
-        <v>46</v>
-      </c>
-      <c r="I4" s="4" t="s">
-        <v>49</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="K4" s="2" t="s">
+      <c r="U4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="V4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="W4" s="2">
+        <v>450</v>
+      </c>
+      <c r="X4" s="2">
+        <v>450</v>
+      </c>
+      <c r="Y4" s="2">
+        <v>450</v>
+      </c>
+      <c r="Z4" s="2">
+        <v>450</v>
+      </c>
+      <c r="AB4" s="2">
+        <v>450</v>
+      </c>
+      <c r="AD4" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="L4" s="3">
-        <v>44197</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="P4" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q4" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="R4" s="3">
-        <v>43831</v>
-      </c>
-      <c r="S4" s="6">
-        <v>1</v>
-      </c>
-      <c r="U4" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="V4" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="W4" s="2">
-        <v>7.5</v>
-      </c>
-      <c r="X4" s="2">
-        <v>7.5</v>
-      </c>
-      <c r="Y4" s="2">
-        <v>7.5</v>
-      </c>
-      <c r="Z4" s="2">
-        <v>7.5</v>
-      </c>
-      <c r="AB4" s="2">
-        <v>7.5</v>
-      </c>
-      <c r="AD4" s="2" t="s">
-        <v>77</v>
-      </c>
       <c r="AH4" s="2" t="s">
-        <v>78</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>33</v>
+        <v>58</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>30</v>
+        <v>61</v>
       </c>
       <c r="C5" s="2">
         <v>1000003</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>24</v>
+        <v>62</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>63</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>27</v>
+        <v>66</v>
       </c>
       <c r="G5" s="2" t="s">
-        <v>44</v>
+        <v>67</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>50</v>
+        <v>68</v>
+      </c>
+      <c r="I5" s="7" t="s">
+        <v>69</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>52</v>
+        <v>30</v>
+      </c>
+      <c r="K5" s="3">
+        <v>45292</v>
       </c>
       <c r="L5" s="3">
-        <v>45292</v>
-      </c>
-      <c r="M5" s="3">
         <v>45658</v>
       </c>
-      <c r="N5" s="2" t="s">
-        <v>56</v>
+      <c r="M5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>37</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>62</v>
+        <v>38</v>
       </c>
       <c r="P5" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q5" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="R5" s="3">
+        <v>40</v>
+      </c>
+      <c r="Q5" s="3">
         <v>43831</v>
       </c>
-      <c r="S5" s="6">
+      <c r="R5" s="5">
         <v>0.75</v>
       </c>
-      <c r="T5" s="3">
+      <c r="S5" s="3">
         <v>45383</v>
       </c>
+      <c r="T5" s="2" t="s">
+        <v>22</v>
+      </c>
       <c r="U5" s="2" t="s">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="V5" s="2" t="s">
-        <v>35</v>
+        <v>6</v>
       </c>
       <c r="W5" s="2">
-        <v>3</v>
+        <v>225</v>
       </c>
       <c r="X5" s="2">
-        <v>3</v>
+        <v>225</v>
       </c>
       <c r="Y5" s="2">
-        <v>3</v>
+        <v>225</v>
       </c>
       <c r="Z5" s="2">
-        <v>4</v>
+        <v>225</v>
       </c>
       <c r="AA5" s="2">
-        <v>4</v>
+        <v>225</v>
       </c>
       <c r="AE5" s="2" t="s">
-        <v>79</v>
+        <v>53</v>
       </c>
       <c r="AF5" s="2" t="s">
-        <v>80</v>
+        <v>54</v>
       </c>
     </row>
   </sheetData>
   <autoFilter ref="A2:AI5" xr:uid="{ED5AB09E-8427-43CE-A5E4-2EA0450F5516}"/>
   <mergeCells count="5">
-    <mergeCell ref="W1:AC1"/>
+    <mergeCell ref="V1:AC1"/>
     <mergeCell ref="A1:F1"/>
-    <mergeCell ref="G1:J1"/>
-    <mergeCell ref="K1:N1"/>
-    <mergeCell ref="O1:V1"/>
+    <mergeCell ref="G1:I1"/>
+    <mergeCell ref="J1:M1"/>
+    <mergeCell ref="N1:U1"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
-  <hyperlinks>
-    <hyperlink ref="I3" r:id="rId1" xr:uid="{B5D074B2-8CC4-48F5-95CB-7157235F9C6D}"/>
-    <hyperlink ref="I4:I5" r:id="rId2" display="demo.manager1@nhs.net" xr:uid="{26B17EC8-D984-4A86-9E31-39AD0ED3D910}"/>
-    <hyperlink ref="I4" r:id="rId3" xr:uid="{ABF5D15B-5A43-4452-BFDA-9BB13AD6335A}"/>
-    <hyperlink ref="I5" r:id="rId4" xr:uid="{BBBAA571-40CB-43F2-8478-BE9EF0AA8E22}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>